<commit_message>
Removed bugs in broken tests. Half done
</commit_message>
<xml_diff>
--- a/resources/ExcelsheetData/ETNATestData.xlsx
+++ b/resources/ExcelsheetData/ETNATestData.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\UnilogProjects\Etna\resources\ExcelsheetData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\UnilogProjects\template\resources\ExcelsheetData\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7365" firstSheet="1" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7365" firstSheet="17" activeTab="18"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet names" sheetId="4" r:id="rId1"/>
@@ -117,7 +117,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1464" uniqueCount="452">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1464" uniqueCount="453">
   <si>
     <t xml:space="preserve">TC No </t>
   </si>
@@ -1193,9 +1193,6 @@
     <t>Please Enter Confirm Password.</t>
   </si>
   <si>
-    <t>Please Enter First Name.Please Enter Last Name.Please Enter Company Name.Please Enter Email Address.Please Enter Password.Please Enter Confirm Password.Please Enter Address 1.Please Enter City Name.Please Select State Name.Please Enter Zipcode.Please Enter Phone Number.</t>
-  </si>
-  <si>
     <t>Please Enter valid email address.</t>
   </si>
   <si>
@@ -1496,6 +1493,12 @@
   </si>
   <si>
     <t>forgotPassword_ES</t>
+  </si>
+  <si>
+    <t>Please enter Address 1.</t>
+  </si>
+  <si>
+    <t>Please Enter First Name.Please Enter Last Name.Please Enter Company Name.Please Enter Email Address.Please Enter Password.Please Enter Confirm Password.Please enter Address 1.Please Enter City Name.Please Select State Name.Please Enter Zipcode.Please Enter Phone Number.</t>
   </si>
 </sst>
 </file>
@@ -1728,7 +1731,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="93">
+  <cellXfs count="92">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -1890,7 +1893,6 @@
     <xf numFmtId="49" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
@@ -2198,26 +2200,26 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="B1" s="15" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="68" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="68" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -2225,7 +2227,7 @@
         <v>52</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -2233,7 +2235,7 @@
         <v>60</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -2241,7 +2243,7 @@
         <v>102</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -2249,7 +2251,7 @@
         <v>88</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -2257,23 +2259,23 @@
         <v>142</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="68" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="68" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -2281,47 +2283,47 @@
         <v>154</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="68" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="68" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="68" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="B14" s="11" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="68" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="B15" s="11" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="68" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="B16" s="11" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -2329,7 +2331,7 @@
         <v>219</v>
       </c>
       <c r="B17" s="11" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -2337,7 +2339,7 @@
         <v>242</v>
       </c>
       <c r="B18" s="11" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -2345,7 +2347,7 @@
         <v>284</v>
       </c>
       <c r="B19" s="11" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
@@ -2353,7 +2355,7 @@
         <v>286</v>
       </c>
       <c r="B20" s="11" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
@@ -2361,31 +2363,31 @@
         <v>351</v>
       </c>
       <c r="B21" s="11" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="68" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="B22" s="11" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="68" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="B23" s="11" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="11" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="B24" s="11" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
   </sheetData>
@@ -3639,7 +3641,7 @@
         <v>12345678</v>
       </c>
       <c r="F9" s="51" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="G9" s="52"/>
       <c r="H9" s="52"/>
@@ -3736,7 +3738,7 @@
         <v>28</v>
       </c>
       <c r="B2" s="89" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="C2" s="88" t="s">
         <v>17</v>
@@ -4235,15 +4237,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView tabSelected="1" topLeftCell="F5" workbookViewId="0">
+      <selection activeCell="N12" sqref="N12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20.42578125" customWidth="1"/>
     <col min="2" max="2" width="25" customWidth="1"/>
-    <col min="3" max="8" width="13" customWidth="1"/>
+    <col min="3" max="4" width="13" customWidth="1"/>
+    <col min="5" max="5" width="24" customWidth="1"/>
+    <col min="6" max="8" width="13" customWidth="1"/>
     <col min="9" max="9" width="42.85546875" customWidth="1"/>
     <col min="13" max="13" width="37.140625" customWidth="1"/>
     <col min="14" max="14" width="30.140625" customWidth="1"/>
@@ -4295,7 +4299,7 @@
     </row>
     <row r="2" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="B2" s="11" t="s">
         <v>17</v>
@@ -4337,7 +4341,7 @@
     </row>
     <row r="3" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="B3" s="11"/>
       <c r="C3" s="11" t="s">
@@ -4379,7 +4383,7 @@
     </row>
     <row r="4" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="B4" s="11" t="s">
         <v>17</v>
@@ -4421,7 +4425,7 @@
     </row>
     <row r="5" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="B5" s="11" t="s">
         <v>17</v>
@@ -4463,7 +4467,7 @@
     </row>
     <row r="6" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B6" s="11" t="s">
         <v>17</v>
@@ -4505,7 +4509,7 @@
     </row>
     <row r="7" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="B7" s="11" t="s">
         <v>17</v>
@@ -4542,12 +4546,12 @@
         <v>81</v>
       </c>
       <c r="N7" s="14" t="s">
-        <v>334</v>
+        <v>451</v>
       </c>
     </row>
     <row r="8" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="B8" s="11" t="s">
         <v>17</v>
@@ -4589,7 +4593,7 @@
     </row>
     <row r="9" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="B9" s="11" t="s">
         <v>17</v>
@@ -4631,7 +4635,7 @@
     </row>
     <row r="10" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="13" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="B10" s="11" t="s">
         <v>17</v>
@@ -4673,7 +4677,7 @@
     </row>
     <row r="11" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="13" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="B11" s="11" t="s">
         <v>17</v>
@@ -4715,7 +4719,7 @@
     </row>
     <row r="12" spans="1:14" ht="167.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="13" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="B12" s="11"/>
       <c r="C12" s="11"/>
@@ -4730,12 +4734,12 @@
       <c r="L12" s="11"/>
       <c r="M12" s="11"/>
       <c r="N12" s="53" t="s">
-        <v>353</v>
+        <v>452</v>
       </c>
     </row>
     <row r="13" spans="1:14" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="13" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="B13" s="11" t="s">
         <v>17</v>
@@ -4779,7 +4783,7 @@
     </row>
     <row r="14" spans="1:14" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="13" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="B14" s="11" t="s">
         <v>17</v>
@@ -4818,12 +4822,12 @@
         <v>23</v>
       </c>
       <c r="N14" s="14" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="15" spans="1:14" ht="69" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="13" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="B15" s="11" t="s">
         <v>17</v>
@@ -4867,7 +4871,7 @@
     </row>
     <row r="16" spans="1:14" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="13" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="B16" s="11" t="s">
         <v>17</v>
@@ -4911,7 +4915,7 @@
     </row>
     <row r="17" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="13" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="B17" s="11" t="s">
         <v>17</v>
@@ -4961,10 +4965,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4973,70 +4977,68 @@
     <col min="2" max="2" width="12.5703125" customWidth="1"/>
     <col min="3" max="3" width="29.5703125" customWidth="1"/>
     <col min="4" max="4" width="61.5703125" customWidth="1"/>
-    <col min="5" max="5" width="43.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="12" t="s">
+        <v>439</v>
+      </c>
+      <c r="C1" s="12" t="s">
         <v>440</v>
-      </c>
-      <c r="C1" s="12" t="s">
-        <v>441</v>
       </c>
       <c r="D1" s="12" t="s">
         <v>109</v>
       </c>
-      <c r="E1" s="91"/>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B2" s="11"/>
       <c r="C2" s="11"/>
       <c r="D2" s="11" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="11" t="s">
         <v>443</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="11" t="s">
-        <v>444</v>
       </c>
       <c r="B3" s="11" t="s">
         <v>17</v>
       </c>
       <c r="C3" s="11"/>
       <c r="D3" s="11" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="11" t="s">
         <v>445</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="11" t="s">
-        <v>446</v>
       </c>
       <c r="B4" s="11"/>
       <c r="C4" s="11" t="s">
         <v>76</v>
       </c>
       <c r="D4" s="11" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="11" t="s">
         <v>447</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="11" t="s">
-        <v>448</v>
       </c>
       <c r="B5" s="11" t="s">
         <v>17</v>
       </c>
       <c r="C5" s="11" t="s">
+        <v>448</v>
+      </c>
+      <c r="D5" s="11" t="s">
         <v>449</v>
-      </c>
-      <c r="D5" s="11" t="s">
-        <v>450</v>
       </c>
     </row>
   </sheetData>
@@ -5046,10 +5048,10 @@
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N21"/>
+  <dimension ref="A1:N17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="19.5" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -5110,7 +5112,7 @@
     </row>
     <row r="2" spans="1:14" ht="54" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="B2" s="11" t="s">
         <v>17</v>
@@ -5152,7 +5154,7 @@
     </row>
     <row r="3" spans="1:14" ht="54" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="B3" s="11"/>
       <c r="C3" s="11" t="s">
@@ -5194,7 +5196,7 @@
     </row>
     <row r="4" spans="1:14" ht="54" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="B4" s="11" t="s">
         <v>17</v>
@@ -5236,7 +5238,7 @@
     </row>
     <row r="5" spans="1:14" ht="54" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="B5" s="11" t="s">
         <v>17</v>
@@ -5278,7 +5280,7 @@
     </row>
     <row r="6" spans="1:14" ht="54" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="B6" s="11" t="s">
         <v>17</v>
@@ -5320,7 +5322,7 @@
     </row>
     <row r="7" spans="1:14" ht="54" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="B7" s="11" t="s">
         <v>17</v>
@@ -5362,7 +5364,7 @@
     </row>
     <row r="8" spans="1:14" ht="54" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="B8" s="11" t="s">
         <v>17</v>
@@ -5404,7 +5406,7 @@
     </row>
     <row r="9" spans="1:14" ht="54" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="B9" s="11" t="s">
         <v>17</v>
@@ -5446,7 +5448,7 @@
     </row>
     <row r="10" spans="1:14" ht="54" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="13" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="B10" s="11" t="s">
         <v>17</v>
@@ -5488,7 +5490,7 @@
     </row>
     <row r="11" spans="1:14" ht="54" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="13" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B11" s="11" t="s">
         <v>17</v>
@@ -5530,7 +5532,7 @@
     </row>
     <row r="12" spans="1:14" ht="79.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="13" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B12" s="11"/>
       <c r="C12" s="11"/>
@@ -5550,7 +5552,7 @@
     </row>
     <row r="13" spans="1:14" ht="54" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="13" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B13" s="11" t="s">
         <v>17</v>
@@ -5594,7 +5596,7 @@
     </row>
     <row r="14" spans="1:14" ht="54" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="13" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B14" s="11" t="s">
         <v>17</v>
@@ -5632,13 +5634,13 @@
       <c r="M14" s="62" t="s">
         <v>23</v>
       </c>
-      <c r="N14" t="s">
+      <c r="N14" s="11" t="s">
         <v>347</v>
       </c>
     </row>
     <row r="15" spans="1:14" ht="54" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="13" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="B15" s="11" t="s">
         <v>17</v>
@@ -5682,7 +5684,7 @@
     </row>
     <row r="16" spans="1:14" ht="54" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="13" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="B16" s="11" t="s">
         <v>17</v>
@@ -5726,7 +5728,7 @@
     </row>
     <row r="17" spans="1:14" ht="54" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="13" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="B17" s="11" t="s">
         <v>17</v>
@@ -5766,10 +5768,6 @@
         <v>350</v>
       </c>
     </row>
-    <row r="18" spans="1:14" ht="54" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="19" spans="1:14" ht="54" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="20" spans="1:14" ht="54" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="21" spans="1:14" ht="54" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A1" location="'Sheet names'!A1" display="password"/>
@@ -6168,12 +6166,12 @@
       <c r="N7" s="2"/>
       <c r="O7" s="2"/>
       <c r="P7" s="65" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="78" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B8" s="11" t="s">
         <v>31</v>
@@ -6212,12 +6210,12 @@
       <c r="N8" s="2"/>
       <c r="O8" s="2"/>
       <c r="P8" s="65" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="78" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="B9" s="11" t="s">
         <v>31</v>
@@ -6256,12 +6254,12 @@
       <c r="N9" s="2"/>
       <c r="O9" s="2"/>
       <c r="P9" s="65" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="78" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="B10" s="11" t="s">
         <v>31</v>
@@ -6300,12 +6298,12 @@
       <c r="N10" s="2"/>
       <c r="O10" s="2"/>
       <c r="P10" s="65" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
     <row r="11" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="78" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="B11" s="11" t="s">
         <v>31</v>
@@ -6349,7 +6347,7 @@
     </row>
     <row r="12" spans="1:16" ht="165" x14ac:dyDescent="0.25">
       <c r="A12" s="79" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="B12" s="85"/>
       <c r="C12" s="82"/>
@@ -6366,12 +6364,12 @@
       <c r="N12" s="2"/>
       <c r="O12" s="2"/>
       <c r="P12" s="66" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="13" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="79" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="B13" s="11" t="s">
         <v>31</v>
@@ -6417,7 +6415,7 @@
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" s="79" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="B14" s="86" t="s">
         <v>17</v>
@@ -6463,7 +6461,7 @@
     </row>
     <row r="15" spans="1:16" ht="60" x14ac:dyDescent="0.25">
       <c r="A15" s="79" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="B15" s="11" t="s">
         <v>31</v>
@@ -6504,12 +6502,12 @@
       <c r="N15" s="2"/>
       <c r="O15" s="2"/>
       <c r="P15" s="65" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
     </row>
     <row r="16" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="79" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B16" s="11" t="s">
         <v>31</v>
@@ -6590,54 +6588,54 @@
         <v>108</v>
       </c>
       <c r="D1" s="15" t="s">
+        <v>367</v>
+      </c>
+      <c r="E1" s="15" t="s">
+        <v>355</v>
+      </c>
+      <c r="F1" s="15" t="s">
         <v>368</v>
       </c>
-      <c r="E1" s="15" t="s">
-        <v>356</v>
-      </c>
-      <c r="F1" s="15" t="s">
+      <c r="G1" s="15" t="s">
         <v>369</v>
-      </c>
-      <c r="G1" s="15" t="s">
-        <v>370</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
+        <v>370</v>
+      </c>
+      <c r="B2" s="13" t="s">
         <v>371</v>
-      </c>
-      <c r="B2" s="13" t="s">
-        <v>372</v>
       </c>
       <c r="C2" s="13" t="s">
         <v>112</v>
       </c>
       <c r="D2" s="11"/>
       <c r="E2" s="13" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="F2" s="11"/>
       <c r="G2" s="11" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="91.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
+        <v>374</v>
+      </c>
+      <c r="B3" s="64" t="s">
         <v>375</v>
-      </c>
-      <c r="B3" s="64" t="s">
-        <v>376</v>
       </c>
       <c r="C3" s="13" t="s">
         <v>112</v>
       </c>
       <c r="D3" s="11"/>
       <c r="E3" s="13" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="F3" s="11"/>
       <c r="G3" s="11" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
     </row>
   </sheetData>
@@ -6672,10 +6670,10 @@
         <v>103</v>
       </c>
       <c r="C1" s="12" t="s">
+        <v>355</v>
+      </c>
+      <c r="D1" s="12" t="s">
         <v>356</v>
-      </c>
-      <c r="D1" s="12" t="s">
-        <v>357</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -6683,13 +6681,13 @@
         <v>127</v>
       </c>
       <c r="B2" s="64" t="s">
+        <v>357</v>
+      </c>
+      <c r="C2" s="13" t="s">
         <v>358</v>
       </c>
-      <c r="C2" s="13" t="s">
+      <c r="D2" s="13" t="s">
         <v>359</v>
-      </c>
-      <c r="D2" s="13" t="s">
-        <v>360</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -6697,10 +6695,10 @@
         <v>130</v>
       </c>
       <c r="B3" s="64" t="s">
+        <v>360</v>
+      </c>
+      <c r="C3" s="11" t="s">
         <v>361</v>
-      </c>
-      <c r="C3" s="11" t="s">
-        <v>362</v>
       </c>
       <c r="D3" s="11"/>
     </row>
@@ -6709,25 +6707,25 @@
         <v>133</v>
       </c>
       <c r="B4" s="64" t="s">
+        <v>362</v>
+      </c>
+      <c r="C4" s="11" t="s">
         <v>363</v>
-      </c>
-      <c r="C4" s="11" t="s">
-        <v>364</v>
       </c>
       <c r="D4" s="11"/>
     </row>
     <row r="5" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
+        <v>364</v>
+      </c>
+      <c r="B5" s="64" t="s">
         <v>365</v>
-      </c>
-      <c r="B5" s="64" t="s">
-        <v>366</v>
       </c>
       <c r="C5" s="13" t="s">
         <v>72</v>
       </c>
       <c r="D5" s="13" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
     </row>
   </sheetData>
@@ -7385,7 +7383,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
@@ -7428,7 +7426,7 @@
       <c r="A3" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="B3" s="92" t="s">
+      <c r="B3" s="91" t="s">
         <v>56</v>
       </c>
       <c r="C3" s="24" t="s">

</xml_diff>

<commit_message>
AND and - Scenarios complete
</commit_message>
<xml_diff>
--- a/resources/ExcelsheetData/ETNATestData.xlsx
+++ b/resources/ExcelsheetData/ETNATestData.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\UnilogProjects\template\resources\ExcelsheetData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\UnilogProjects\Etna\resources\ExcelsheetData\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7365" firstSheet="17" activeTab="18"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7365" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet names" sheetId="4" r:id="rId1"/>
@@ -3977,7 +3977,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
@@ -4237,7 +4239,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F5" workbookViewId="0">
+    <sheetView topLeftCell="F5" workbookViewId="0">
       <selection activeCell="N12" sqref="N12"/>
     </sheetView>
   </sheetViews>
@@ -7050,7 +7052,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="33" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>

<commit_message>
Save Cart Module Updated
</commit_message>
<xml_diff>
--- a/resources/ExcelsheetData/ETNATestData.xlsx
+++ b/resources/ExcelsheetData/ETNATestData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7365" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7365" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet names" sheetId="4" r:id="rId1"/>
@@ -17,29 +17,30 @@
     <sheet name="addAndDeleteNew_GU_SU_APA" sheetId="1" r:id="rId3"/>
     <sheet name="login_ErrorScenarios" sheetId="3" r:id="rId4"/>
     <sheet name="orderFullFillmentFlow" sheetId="6" r:id="rId5"/>
-    <sheet name="orderFullFillment_ES" sheetId="7" r:id="rId6"/>
-    <sheet name="loginAs_SU_PA_GU" sheetId="5" r:id="rId7"/>
-    <sheet name="rFQ_FN_LN_PN_Email_ES" sheetId="8" r:id="rId8"/>
-    <sheet name="signedUser_cpnPDP_ES" sheetId="9" r:id="rId9"/>
-    <sheet name="ShareFunctionality" sheetId="10" r:id="rId10"/>
-    <sheet name="ShareFunctionality_ES" sheetId="11" r:id="rId11"/>
-    <sheet name="verifyContentsOfFooterLinks" sheetId="15" r:id="rId12"/>
-    <sheet name="verifyContactUsPositives" sheetId="14" r:id="rId13"/>
-    <sheet name="verifyContactUsPageES" sheetId="13" r:id="rId14"/>
-    <sheet name="verify_Disable_PADPA" sheetId="12" r:id="rId15"/>
-    <sheet name="verifyContentsOfHeaderLinks" sheetId="16" r:id="rId16"/>
-    <sheet name="sC_BulkAlert_ItemNotChosen" sheetId="18" r:id="rId17"/>
-    <sheet name="verifyFirstTimeOrderingRegES" sheetId="19" r:id="rId18"/>
-    <sheet name="verifyNewRURegistrationES" sheetId="21" r:id="rId19"/>
-    <sheet name="verifyNewCCUserRegistrationES" sheetId="20" r:id="rId20"/>
-    <sheet name="pG_bulkAlert_ItemNotChosen" sheetId="17" r:id="rId21"/>
-    <sheet name="addNewPA_errorScenarios" sheetId="24" r:id="rId22"/>
-    <sheet name="rFQ_PositiveFlow" sheetId="23" r:id="rId23"/>
-    <sheet name="rFQ_quantityField_ES" sheetId="22" r:id="rId24"/>
+    <sheet name="verifyEditCartName_ES_PS" sheetId="26" r:id="rId6"/>
+    <sheet name="orderFullFillment_ES" sheetId="7" r:id="rId7"/>
+    <sheet name="loginAs_SU_PA_GU" sheetId="5" r:id="rId8"/>
+    <sheet name="rFQ_FN_LN_PN_Email_ES" sheetId="8" r:id="rId9"/>
+    <sheet name="signedUser_cpnPDP_ES" sheetId="9" r:id="rId10"/>
+    <sheet name="ShareFunctionality" sheetId="10" r:id="rId11"/>
+    <sheet name="ShareFunctionality_ES" sheetId="11" r:id="rId12"/>
+    <sheet name="verifyContentsOfFooterLinks" sheetId="15" r:id="rId13"/>
+    <sheet name="verifyContactUsPositives" sheetId="14" r:id="rId14"/>
+    <sheet name="verifyContactUsPageES" sheetId="13" r:id="rId15"/>
+    <sheet name="verify_Disable_PADPA" sheetId="12" r:id="rId16"/>
+    <sheet name="verifyContentsOfHeaderLinks" sheetId="16" r:id="rId17"/>
+    <sheet name="sC_BulkAlert_ItemNotChosen" sheetId="18" r:id="rId18"/>
+    <sheet name="verifyFirstTimeOrderingRegES" sheetId="19" r:id="rId19"/>
+    <sheet name="verifyNewRURegistrationES" sheetId="21" r:id="rId20"/>
+    <sheet name="verifyNewCCUserRegistrationES" sheetId="20" r:id="rId21"/>
+    <sheet name="pG_bulkAlert_ItemNotChosen" sheetId="17" r:id="rId22"/>
+    <sheet name="addNewPA_errorScenarios" sheetId="24" r:id="rId23"/>
+    <sheet name="rFQ_PositiveFlow" sheetId="23" r:id="rId24"/>
+    <sheet name="rFQ_quantityField_ES" sheetId="22" r:id="rId25"/>
   </sheets>
   <definedNames>
     <definedName name="RegistrationErrorScenarios" localSheetId="3">login_ErrorScenarios!$B$1:$C$2</definedName>
-    <definedName name="RegistrationErrorScenarios" localSheetId="6">loginAs_SU_PA_GU!$B$1:$C$2</definedName>
+    <definedName name="RegistrationErrorScenarios" localSheetId="7">loginAs_SU_PA_GU!$B$1:$C$2</definedName>
     <definedName name="RegistrationErrorScenarios" localSheetId="4">orderFullFillmentFlow!$B$1:$C$1</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
@@ -117,7 +118,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1464" uniqueCount="453">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1479" uniqueCount="466">
   <si>
     <t xml:space="preserve">TC No </t>
   </si>
@@ -1499,6 +1500,45 @@
   </si>
   <si>
     <t>Please Enter First Name.Please Enter Last Name.Please Enter Company Name.Please Enter Email Address.Please Enter Password.Please Enter Confirm Password.Please enter Address 1.Please Enter City Name.Please Select State Name.Please Enter Zipcode.Please Enter Phone Number.</t>
+  </si>
+  <si>
+    <t>TestCase_ID</t>
+  </si>
+  <si>
+    <t>SaveCartName</t>
+  </si>
+  <si>
+    <t>EditCartName</t>
+  </si>
+  <si>
+    <t>ExpectedAlertText</t>
+  </si>
+  <si>
+    <t>TC_SavedCart_001</t>
+  </si>
+  <si>
+    <t>Varsha</t>
+  </si>
+  <si>
+    <t>Varsha123</t>
+  </si>
+  <si>
+    <t>Cart Name Changed</t>
+  </si>
+  <si>
+    <t>TC_SavedCart_002</t>
+  </si>
+  <si>
+    <t>Test Varsha</t>
+  </si>
+  <si>
+    <t>No Changes In Cart Name</t>
+  </si>
+  <si>
+    <t>TC_SavedCart_003</t>
+  </si>
+  <si>
+    <t>Please Enter Cart Name</t>
   </si>
 </sst>
 </file>
@@ -2424,6 +2464,82 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.28515625" customWidth="1"/>
+    <col min="2" max="2" width="23.7109375" customWidth="1"/>
+    <col min="3" max="3" width="65.42578125" style="38" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="72" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="34" t="s">
+        <v>143</v>
+      </c>
+      <c r="C1" s="37" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="17" t="s">
+        <v>145</v>
+      </c>
+      <c r="B2" s="19" t="s">
+        <v>146</v>
+      </c>
+      <c r="C2" s="21" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="17" t="s">
+        <v>148</v>
+      </c>
+      <c r="B3" s="19" t="s">
+        <v>149</v>
+      </c>
+      <c r="C3" s="21" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="17" t="s">
+        <v>150</v>
+      </c>
+      <c r="B4" t="s">
+        <v>151</v>
+      </c>
+      <c r="C4" s="21" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="17" t="s">
+        <v>152</v>
+      </c>
+      <c r="B5" s="19" t="s">
+        <v>153</v>
+      </c>
+      <c r="C5" s="21" t="s">
+        <v>147</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A1" location="'Sheet names'!A1" display="TC No "/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -2486,7 +2602,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G11"/>
   <sheetViews>
@@ -2742,7 +2858,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E10"/>
   <sheetViews>
@@ -2932,7 +3048,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O9"/>
   <sheetViews>
@@ -3360,7 +3476,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O13"/>
   <sheetViews>
@@ -3671,7 +3787,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O2"/>
   <sheetViews>
@@ -3784,7 +3900,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E6"/>
   <sheetViews>
@@ -3907,7 +4023,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C4"/>
   <sheetViews>
@@ -3973,7 +4089,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H10"/>
   <sheetViews>
@@ -4230,736 +4346,6 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A1" location="'Sheet names'!A1" display="TC No "/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N17"/>
-  <sheetViews>
-    <sheetView topLeftCell="F5" workbookViewId="0">
-      <selection activeCell="N12" sqref="N12"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="21" customHeight="1" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="20.42578125" customWidth="1"/>
-    <col min="2" max="2" width="25" customWidth="1"/>
-    <col min="3" max="4" width="13" customWidth="1"/>
-    <col min="5" max="5" width="24" customWidth="1"/>
-    <col min="6" max="8" width="13" customWidth="1"/>
-    <col min="9" max="9" width="42.85546875" customWidth="1"/>
-    <col min="13" max="13" width="37.140625" customWidth="1"/>
-    <col min="14" max="14" width="30.140625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="12" t="s">
-        <v>104</v>
-      </c>
-      <c r="C1" s="12" t="s">
-        <v>105</v>
-      </c>
-      <c r="D1" s="12" t="s">
-        <v>189</v>
-      </c>
-      <c r="E1" s="12" t="s">
-        <v>188</v>
-      </c>
-      <c r="F1" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="12" t="s">
-        <v>303</v>
-      </c>
-      <c r="H1" s="12" t="s">
-        <v>225</v>
-      </c>
-      <c r="I1" s="12" t="s">
-        <v>229</v>
-      </c>
-      <c r="J1" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="K1" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="L1" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="M1" s="12" t="s">
-        <v>106</v>
-      </c>
-      <c r="N1" s="12" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="13" t="s">
-        <v>407</v>
-      </c>
-      <c r="B2" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="C2" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="D2" s="11" t="s">
-        <v>95</v>
-      </c>
-      <c r="E2" s="11"/>
-      <c r="F2" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="G2" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="H2" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="I2" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="J2" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="K2" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="L2" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="M2" s="62" t="s">
-        <v>23</v>
-      </c>
-      <c r="N2" s="14" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="13" t="s">
-        <v>408</v>
-      </c>
-      <c r="B3" s="11"/>
-      <c r="C3" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="D3" s="11" t="s">
-        <v>95</v>
-      </c>
-      <c r="E3" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="F3" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="G3" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="H3" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="I3" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="J3" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="K3" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="L3" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="M3" s="62" t="s">
-        <v>326</v>
-      </c>
-      <c r="N3" s="14" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="13" t="s">
-        <v>409</v>
-      </c>
-      <c r="B4" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="C4" s="11"/>
-      <c r="D4" s="11" t="s">
-        <v>95</v>
-      </c>
-      <c r="E4" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="F4" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="G4" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="H4" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="I4" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="J4" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="K4" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="L4" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="M4" s="62" t="s">
-        <v>327</v>
-      </c>
-      <c r="N4" s="14" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="13" t="s">
-        <v>410</v>
-      </c>
-      <c r="B5" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="C5" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="D5" s="11" t="s">
-        <v>95</v>
-      </c>
-      <c r="E5" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="F5" s="11"/>
-      <c r="G5" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="H5" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="I5" s="11" t="s">
-        <v>328</v>
-      </c>
-      <c r="J5" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="K5" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="L5" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="M5" s="62" t="s">
-        <v>329</v>
-      </c>
-      <c r="N5" s="14" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="13" t="s">
-        <v>411</v>
-      </c>
-      <c r="B6" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="C6" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="D6" s="11" t="s">
-        <v>95</v>
-      </c>
-      <c r="E6" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="F6" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="G6" s="11"/>
-      <c r="H6" s="11" t="s">
-        <v>328</v>
-      </c>
-      <c r="I6" s="11" t="s">
-        <v>331</v>
-      </c>
-      <c r="J6" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="K6" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="L6" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="M6" s="62" t="s">
-        <v>73</v>
-      </c>
-      <c r="N6" s="14" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="13" t="s">
-        <v>412</v>
-      </c>
-      <c r="B7" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="C7" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="D7" s="11" t="s">
-        <v>95</v>
-      </c>
-      <c r="E7" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="F7" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="G7" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="H7" s="11"/>
-      <c r="I7" s="11" t="s">
-        <v>333</v>
-      </c>
-      <c r="J7" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="K7" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="L7" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="M7" s="62" t="s">
-        <v>81</v>
-      </c>
-      <c r="N7" s="14" t="s">
-        <v>451</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="13" t="s">
-        <v>413</v>
-      </c>
-      <c r="B8" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="C8" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="D8" s="11" t="s">
-        <v>95</v>
-      </c>
-      <c r="E8" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="F8" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="G8" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="H8" s="11" t="s">
-        <v>333</v>
-      </c>
-      <c r="I8" s="11" t="s">
-        <v>335</v>
-      </c>
-      <c r="J8" s="11"/>
-      <c r="K8" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="L8" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="M8" s="62" t="s">
-        <v>336</v>
-      </c>
-      <c r="N8" s="14" t="s">
-        <v>337</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="13" t="s">
-        <v>414</v>
-      </c>
-      <c r="B9" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="C9" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="D9" s="11" t="s">
-        <v>95</v>
-      </c>
-      <c r="E9" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="F9" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="G9" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="H9" s="11" t="s">
-        <v>335</v>
-      </c>
-      <c r="I9" s="11" t="s">
-        <v>338</v>
-      </c>
-      <c r="J9" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="K9" s="11"/>
-      <c r="L9" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="M9" s="62" t="s">
-        <v>339</v>
-      </c>
-      <c r="N9" s="14" t="s">
-        <v>340</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="13" t="s">
-        <v>415</v>
-      </c>
-      <c r="B10" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="C10" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="D10" s="11" t="s">
-        <v>95</v>
-      </c>
-      <c r="E10" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="F10" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="G10" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="H10" s="11" t="s">
-        <v>338</v>
-      </c>
-      <c r="I10" s="11" t="s">
-        <v>341</v>
-      </c>
-      <c r="J10" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="K10" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="L10" s="11"/>
-      <c r="M10" s="62" t="s">
-        <v>342</v>
-      </c>
-      <c r="N10" s="14" t="s">
-        <v>343</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="13" t="s">
-        <v>416</v>
-      </c>
-      <c r="B11" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="C11" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="D11" s="11" t="s">
-        <v>95</v>
-      </c>
-      <c r="E11" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="F11" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="G11" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="H11" s="11" t="s">
-        <v>341</v>
-      </c>
-      <c r="I11" s="11" t="s">
-        <v>344</v>
-      </c>
-      <c r="J11" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="K11" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="L11" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="M11" s="11"/>
-      <c r="N11" s="14" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" ht="167.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="13" t="s">
-        <v>417</v>
-      </c>
-      <c r="B12" s="11"/>
-      <c r="C12" s="11"/>
-      <c r="D12" s="11"/>
-      <c r="E12" s="11"/>
-      <c r="F12" s="11"/>
-      <c r="G12" s="11"/>
-      <c r="H12" s="11"/>
-      <c r="I12" s="11"/>
-      <c r="J12" s="11"/>
-      <c r="K12" s="11"/>
-      <c r="L12" s="11"/>
-      <c r="M12" s="11"/>
-      <c r="N12" s="53" t="s">
-        <v>452</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="13" t="s">
-        <v>418</v>
-      </c>
-      <c r="B13" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="C13" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="D13" s="11" t="s">
-        <v>95</v>
-      </c>
-      <c r="E13" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="F13" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="G13" s="11" t="s">
-        <v>318</v>
-      </c>
-      <c r="H13" s="11" t="s">
-        <v>341</v>
-      </c>
-      <c r="I13" s="11" t="s">
-        <v>344</v>
-      </c>
-      <c r="J13" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="K13" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="L13" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="M13" s="62" t="s">
-        <v>23</v>
-      </c>
-      <c r="N13" s="14" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="13" t="s">
-        <v>419</v>
-      </c>
-      <c r="B14" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="C14" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="D14" s="11" t="s">
-        <v>95</v>
-      </c>
-      <c r="E14" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="F14" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="G14" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="H14" s="11" t="s">
-        <v>341</v>
-      </c>
-      <c r="I14" s="11" t="s">
-        <v>344</v>
-      </c>
-      <c r="J14" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="K14" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="L14" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="M14" s="62" t="s">
-        <v>23</v>
-      </c>
-      <c r="N14" s="14" t="s">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14" ht="69" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="13" t="s">
-        <v>420</v>
-      </c>
-      <c r="B15" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="C15" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="D15" s="11" t="s">
-        <v>95</v>
-      </c>
-      <c r="E15" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="F15" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="G15" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="H15" s="11" t="s">
-        <v>341</v>
-      </c>
-      <c r="I15" s="11" t="s">
-        <v>344</v>
-      </c>
-      <c r="J15" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="K15" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="L15" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="M15" s="62" t="s">
-        <v>348</v>
-      </c>
-      <c r="N15" s="14" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="13" t="s">
-        <v>421</v>
-      </c>
-      <c r="B16" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="C16" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="D16" s="11" t="s">
-        <v>95</v>
-      </c>
-      <c r="E16" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="F16" s="11" t="s">
-        <v>323</v>
-      </c>
-      <c r="G16" s="11" t="s">
-        <v>323</v>
-      </c>
-      <c r="H16" s="11" t="s">
-        <v>341</v>
-      </c>
-      <c r="I16" s="11" t="s">
-        <v>344</v>
-      </c>
-      <c r="J16" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="K16" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="L16" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="M16" s="62" t="s">
-        <v>23</v>
-      </c>
-      <c r="N16" s="14" t="s">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="17" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="13" t="s">
-        <v>422</v>
-      </c>
-      <c r="B17" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="C17" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="D17" s="11"/>
-      <c r="E17" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="F17" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="G17" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="H17" s="11" t="s">
-        <v>341</v>
-      </c>
-      <c r="I17" s="11" t="s">
-        <v>344</v>
-      </c>
-      <c r="J17" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="K17" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="L17" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="M17" s="62" t="s">
-        <v>23</v>
-      </c>
-      <c r="N17" s="14" t="s">
-        <v>350</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A1" location="'Sheet names'!A1" display="password"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5052,6 +4438,736 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N17"/>
   <sheetViews>
+    <sheetView topLeftCell="F5" workbookViewId="0">
+      <selection activeCell="N12" sqref="N12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="21" customHeight="1" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="20.42578125" customWidth="1"/>
+    <col min="2" max="2" width="25" customWidth="1"/>
+    <col min="3" max="4" width="13" customWidth="1"/>
+    <col min="5" max="5" width="24" customWidth="1"/>
+    <col min="6" max="8" width="13" customWidth="1"/>
+    <col min="9" max="9" width="42.85546875" customWidth="1"/>
+    <col min="13" max="13" width="37.140625" customWidth="1"/>
+    <col min="14" max="14" width="30.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>104</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>105</v>
+      </c>
+      <c r="D1" s="12" t="s">
+        <v>189</v>
+      </c>
+      <c r="E1" s="12" t="s">
+        <v>188</v>
+      </c>
+      <c r="F1" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="12" t="s">
+        <v>303</v>
+      </c>
+      <c r="H1" s="12" t="s">
+        <v>225</v>
+      </c>
+      <c r="I1" s="12" t="s">
+        <v>229</v>
+      </c>
+      <c r="J1" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" s="12" t="s">
+        <v>106</v>
+      </c>
+      <c r="N1" s="12" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="13" t="s">
+        <v>407</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="G2" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="H2" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="I2" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="J2" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="K2" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="L2" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="M2" s="62" t="s">
+        <v>23</v>
+      </c>
+      <c r="N2" s="14" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="13" t="s">
+        <v>408</v>
+      </c>
+      <c r="B3" s="11"/>
+      <c r="C3" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="E3" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="G3" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="H3" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="I3" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="J3" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="K3" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="L3" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="M3" s="62" t="s">
+        <v>326</v>
+      </c>
+      <c r="N3" s="14" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="13" t="s">
+        <v>409</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" s="11"/>
+      <c r="D4" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="E4" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="G4" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="H4" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="I4" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="J4" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="K4" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="L4" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="M4" s="62" t="s">
+        <v>327</v>
+      </c>
+      <c r="N4" s="14" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="13" t="s">
+        <v>410</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="E5" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="F5" s="11"/>
+      <c r="G5" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="H5" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="I5" s="11" t="s">
+        <v>328</v>
+      </c>
+      <c r="J5" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="K5" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="L5" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="M5" s="62" t="s">
+        <v>329</v>
+      </c>
+      <c r="N5" s="14" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="13" t="s">
+        <v>411</v>
+      </c>
+      <c r="B6" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="E6" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="F6" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="G6" s="11"/>
+      <c r="H6" s="11" t="s">
+        <v>328</v>
+      </c>
+      <c r="I6" s="11" t="s">
+        <v>331</v>
+      </c>
+      <c r="J6" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="K6" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="L6" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="M6" s="62" t="s">
+        <v>73</v>
+      </c>
+      <c r="N6" s="14" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="13" t="s">
+        <v>412</v>
+      </c>
+      <c r="B7" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="E7" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="F7" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="G7" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="H7" s="11"/>
+      <c r="I7" s="11" t="s">
+        <v>333</v>
+      </c>
+      <c r="J7" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="K7" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="L7" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="M7" s="62" t="s">
+        <v>81</v>
+      </c>
+      <c r="N7" s="14" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="13" t="s">
+        <v>413</v>
+      </c>
+      <c r="B8" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="D8" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="E8" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="F8" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="G8" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="H8" s="11" t="s">
+        <v>333</v>
+      </c>
+      <c r="I8" s="11" t="s">
+        <v>335</v>
+      </c>
+      <c r="J8" s="11"/>
+      <c r="K8" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="L8" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="M8" s="62" t="s">
+        <v>336</v>
+      </c>
+      <c r="N8" s="14" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="13" t="s">
+        <v>414</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="E9" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="F9" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="G9" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="H9" s="11" t="s">
+        <v>335</v>
+      </c>
+      <c r="I9" s="11" t="s">
+        <v>338</v>
+      </c>
+      <c r="J9" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="K9" s="11"/>
+      <c r="L9" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="M9" s="62" t="s">
+        <v>339</v>
+      </c>
+      <c r="N9" s="14" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="13" t="s">
+        <v>415</v>
+      </c>
+      <c r="B10" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="C10" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="D10" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="E10" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="F10" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="G10" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="H10" s="11" t="s">
+        <v>338</v>
+      </c>
+      <c r="I10" s="11" t="s">
+        <v>341</v>
+      </c>
+      <c r="J10" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="K10" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="L10" s="11"/>
+      <c r="M10" s="62" t="s">
+        <v>342</v>
+      </c>
+      <c r="N10" s="14" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="13" t="s">
+        <v>416</v>
+      </c>
+      <c r="B11" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="C11" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="D11" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="E11" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="F11" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="G11" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="H11" s="11" t="s">
+        <v>341</v>
+      </c>
+      <c r="I11" s="11" t="s">
+        <v>344</v>
+      </c>
+      <c r="J11" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="K11" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="L11" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="M11" s="11"/>
+      <c r="N11" s="14" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" ht="167.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="13" t="s">
+        <v>417</v>
+      </c>
+      <c r="B12" s="11"/>
+      <c r="C12" s="11"/>
+      <c r="D12" s="11"/>
+      <c r="E12" s="11"/>
+      <c r="F12" s="11"/>
+      <c r="G12" s="11"/>
+      <c r="H12" s="11"/>
+      <c r="I12" s="11"/>
+      <c r="J12" s="11"/>
+      <c r="K12" s="11"/>
+      <c r="L12" s="11"/>
+      <c r="M12" s="11"/>
+      <c r="N12" s="53" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="13" t="s">
+        <v>418</v>
+      </c>
+      <c r="B13" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="C13" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="D13" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="E13" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="F13" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="G13" s="11" t="s">
+        <v>318</v>
+      </c>
+      <c r="H13" s="11" t="s">
+        <v>341</v>
+      </c>
+      <c r="I13" s="11" t="s">
+        <v>344</v>
+      </c>
+      <c r="J13" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="K13" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="L13" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="M13" s="62" t="s">
+        <v>23</v>
+      </c>
+      <c r="N13" s="14" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="13" t="s">
+        <v>419</v>
+      </c>
+      <c r="B14" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="C14" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="D14" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="E14" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="F14" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="G14" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="H14" s="11" t="s">
+        <v>341</v>
+      </c>
+      <c r="I14" s="11" t="s">
+        <v>344</v>
+      </c>
+      <c r="J14" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="K14" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="L14" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="M14" s="62" t="s">
+        <v>23</v>
+      </c>
+      <c r="N14" s="14" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" ht="69" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="13" t="s">
+        <v>420</v>
+      </c>
+      <c r="B15" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="C15" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="D15" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="E15" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="F15" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="G15" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="H15" s="11" t="s">
+        <v>341</v>
+      </c>
+      <c r="I15" s="11" t="s">
+        <v>344</v>
+      </c>
+      <c r="J15" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="K15" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="L15" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="M15" s="62" t="s">
+        <v>348</v>
+      </c>
+      <c r="N15" s="14" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="13" t="s">
+        <v>421</v>
+      </c>
+      <c r="B16" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="C16" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="D16" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="E16" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="F16" s="11" t="s">
+        <v>323</v>
+      </c>
+      <c r="G16" s="11" t="s">
+        <v>323</v>
+      </c>
+      <c r="H16" s="11" t="s">
+        <v>341</v>
+      </c>
+      <c r="I16" s="11" t="s">
+        <v>344</v>
+      </c>
+      <c r="J16" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="K16" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="L16" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="M16" s="62" t="s">
+        <v>23</v>
+      </c>
+      <c r="N16" s="14" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="13" t="s">
+        <v>422</v>
+      </c>
+      <c r="B17" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="C17" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="D17" s="11"/>
+      <c r="E17" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="F17" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="G17" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="H17" s="11" t="s">
+        <v>341</v>
+      </c>
+      <c r="I17" s="11" t="s">
+        <v>344</v>
+      </c>
+      <c r="J17" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="K17" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="L17" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="M17" s="62" t="s">
+        <v>23</v>
+      </c>
+      <c r="N17" s="14" t="s">
+        <v>350</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A1" location="'Sheet names'!A1" display="password"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:N17"/>
+  <sheetViews>
     <sheetView topLeftCell="A15" workbookViewId="0">
       <selection activeCell="B16" sqref="B16"/>
     </sheetView>
@@ -5778,7 +5894,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C4"/>
   <sheetViews>
@@ -5843,7 +5959,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P16"/>
   <sheetViews>
@@ -6562,7 +6678,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G3"/>
   <sheetViews>
@@ -6648,7 +6764,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D5"/>
   <sheetViews>
@@ -7052,7 +7168,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="33" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
@@ -7284,6 +7400,82 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21" customWidth="1"/>
+    <col min="2" max="2" width="21.5703125" customWidth="1"/>
+    <col min="3" max="3" width="22.28515625" customWidth="1"/>
+    <col min="4" max="4" width="28.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="15" t="s">
+        <v>453</v>
+      </c>
+      <c r="B1" s="15" t="s">
+        <v>454</v>
+      </c>
+      <c r="C1" s="15" t="s">
+        <v>455</v>
+      </c>
+      <c r="D1" s="15" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="11" t="s">
+        <v>457</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>458</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>459</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="11" t="s">
+        <v>461</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>462</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>462</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="11" t="s">
+        <v>464</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>458</v>
+      </c>
+      <c r="C4" s="11"/>
+      <c r="D4" s="11" t="s">
+        <v>465</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E5"/>
   <sheetViews>
@@ -7381,7 +7573,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D4"/>
   <sheetViews>
@@ -7461,7 +7653,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H10"/>
   <sheetViews>
@@ -7728,80 +7920,4 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="15.28515625" customWidth="1"/>
-    <col min="2" max="2" width="23.7109375" customWidth="1"/>
-    <col min="3" max="3" width="65.42578125" style="38" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="72" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="34" t="s">
-        <v>143</v>
-      </c>
-      <c r="C1" s="37" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="17" t="s">
-        <v>145</v>
-      </c>
-      <c r="B2" s="19" t="s">
-        <v>146</v>
-      </c>
-      <c r="C2" s="21" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="17" t="s">
-        <v>148</v>
-      </c>
-      <c r="B3" s="19" t="s">
-        <v>149</v>
-      </c>
-      <c r="C3" s="21" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="17" t="s">
-        <v>150</v>
-      </c>
-      <c r="B4" t="s">
-        <v>151</v>
-      </c>
-      <c r="C4" s="21" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="17" t="s">
-        <v>152</v>
-      </c>
-      <c r="B5" s="19" t="s">
-        <v>153</v>
-      </c>
-      <c r="C5" s="21" t="s">
-        <v>147</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A1" location="'Sheet names'!A1" display="TC No "/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Added verification of UOM in my cart page
</commit_message>
<xml_diff>
--- a/resources/ExcelsheetData/ETNATestData.xlsx
+++ b/resources/ExcelsheetData/ETNATestData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7365" firstSheet="16" activeTab="16"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7365" firstSheet="4" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet names" sheetId="4" r:id="rId1"/>
@@ -3863,7 +3863,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:O2"/>
     </sheetView>
   </sheetViews>
@@ -7077,7 +7077,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="33" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>

<commit_message>
Completed all the tests that are in standard
</commit_message>
<xml_diff>
--- a/resources/ExcelsheetData/ETNATestData.xlsx
+++ b/resources/ExcelsheetData/ETNATestData.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26215"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\UnilogProjects\Etna\resources\ExcelsheetData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hemanthsridhar/Projects/UnilogProjects/template/resources/ExcelsheetData/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7365" firstSheet="21" activeTab="24"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16480" firstSheet="19" activeTab="25"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet names" sheetId="4" r:id="rId1"/>
@@ -37,8 +37,9 @@
     <sheet name="pG_bulkAlert_ItemNotChosen" sheetId="17" r:id="rId23"/>
     <sheet name="addNewPA_errorScenarios" sheetId="24" r:id="rId24"/>
     <sheet name="editContact_ES" sheetId="30" r:id="rId25"/>
-    <sheet name="rFQ_PositiveFlow" sheetId="23" r:id="rId26"/>
-    <sheet name="rFQ_quantityField_ES" sheetId="22" r:id="rId27"/>
+    <sheet name="cartFileUploadDifferentFormats" sheetId="31" r:id="rId26"/>
+    <sheet name="rFQ_PositiveFlow" sheetId="23" r:id="rId27"/>
+    <sheet name="rFQ_quantityField_ES" sheetId="22" r:id="rId28"/>
   </sheets>
   <definedNames>
     <definedName name="RegistrationErrorScenarios" localSheetId="3">login_ErrorScenarios!$B$1:$C$2</definedName>
@@ -46,9 +47,12 @@
     <definedName name="RegistrationErrorScenarios" localSheetId="4">orderFullFillmentFlow!$B$1:$C$1</definedName>
     <definedName name="RegistrationErrorScenarios" localSheetId="5">pG_PLPInPopUp_ES!#REF!</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -121,7 +125,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1611" uniqueCount="511">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1632" uniqueCount="521">
   <si>
     <t xml:space="preserve">TC No </t>
   </si>
@@ -1672,12 +1676,42 @@
   <si>
     <t>Verification of 'Edit Contact' functionality when invalid phone number is entered</t>
   </si>
+  <si>
+    <t>TC_QOP_028</t>
+  </si>
+  <si>
+    <t>pathToTheInvalidFile</t>
+  </si>
+  <si>
+    <t>selectXLSXFileToUploadAlertMessage</t>
+  </si>
+  <si>
+    <t>Please upload .xlsx file.</t>
+  </si>
+  <si>
+    <t>resources/TestData/FileUpload.xls</t>
+  </si>
+  <si>
+    <t>resources/TestData/docFileForCartFileUpload.doc</t>
+  </si>
+  <si>
+    <t>resources/TestData/docxFileForCartFileUpload.docx</t>
+  </si>
+  <si>
+    <t>resources/TestData/tabDelimited.txt</t>
+  </si>
+  <si>
+    <t>resources/TestData/commaSeperated.csv</t>
+  </si>
+  <si>
+    <t>resources/TestData/testdata.png</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1769,6 +1803,26 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -1821,16 +1875,16 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1893,7 +1947,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="101">
+  <cellXfs count="106">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -2073,6 +2127,19 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="3" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
   </cellXfs>
@@ -2370,131 +2437,129 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A24"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="34.140625" customWidth="1"/>
+    <col min="1" max="1" width="34.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" s="15" t="s">
         <v>353</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" s="60" t="s">
         <v>359</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" s="60" t="s">
         <v>352</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A4" s="60" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A5" s="60" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A6" s="60" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A7" s="60" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A8" s="60" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A9" s="60" t="s">
         <v>354</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A10" s="60" t="s">
         <v>355</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A11" s="60" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A12" s="60" t="s">
         <v>360</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A13" s="60" t="s">
         <v>361</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A14" s="60" t="s">
         <v>356</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A15" s="60" t="s">
         <v>362</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A16" s="60" t="s">
         <v>363</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A17" s="60" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A18" s="60" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A19" s="60" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A20" s="60" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A21" s="60" t="s">
         <v>312</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A22" s="60" t="s">
         <v>315</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A23" s="60" t="s">
         <v>357</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A24" s="11" t="s">
         <v>375</v>
       </c>
@@ -2537,17 +2602,17 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.42578125" customWidth="1"/>
-    <col min="2" max="2" width="47.28515625" style="34" customWidth="1"/>
-    <col min="4" max="4" width="17.140625" customWidth="1"/>
-    <col min="6" max="6" width="28.5703125" customWidth="1"/>
-    <col min="7" max="7" width="26.140625" customWidth="1"/>
-    <col min="8" max="8" width="50.85546875" customWidth="1"/>
+    <col min="1" max="1" width="15.5" customWidth="1"/>
+    <col min="2" max="2" width="47.33203125" style="34" customWidth="1"/>
+    <col min="4" max="4" width="17.1640625" customWidth="1"/>
+    <col min="6" max="6" width="28.5" customWidth="1"/>
+    <col min="7" max="7" width="26.1640625" customWidth="1"/>
+    <col min="8" max="8" width="50.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="64" t="s">
         <v>0</v>
       </c>
@@ -2573,7 +2638,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="30" x14ac:dyDescent="0.2">
       <c r="A2" s="16" t="s">
         <v>109</v>
       </c>
@@ -2591,7 +2656,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="16" t="s">
         <v>113</v>
       </c>
@@ -2615,7 +2680,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="16" t="s">
         <v>120</v>
       </c>
@@ -2639,7 +2704,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="16" t="s">
         <v>123</v>
       </c>
@@ -2663,7 +2728,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="16" t="s">
         <v>126</v>
       </c>
@@ -2687,7 +2752,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="16" t="s">
         <v>129</v>
       </c>
@@ -2711,7 +2776,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="30" x14ac:dyDescent="0.2">
       <c r="A8" s="16" t="s">
         <v>132</v>
       </c>
@@ -2737,7 +2802,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" ht="30" x14ac:dyDescent="0.2">
       <c r="A9" s="16" t="s">
         <v>136</v>
       </c>
@@ -2763,7 +2828,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" ht="30" x14ac:dyDescent="0.2">
       <c r="A10" s="16" t="s">
         <v>120</v>
       </c>
@@ -2806,14 +2871,14 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.28515625" customWidth="1"/>
-    <col min="2" max="2" width="23.7109375" customWidth="1"/>
-    <col min="3" max="3" width="65.42578125" style="34" customWidth="1"/>
+    <col min="1" max="1" width="15.33203125" customWidth="1"/>
+    <col min="2" max="2" width="23.6640625" customWidth="1"/>
+    <col min="3" max="3" width="65.5" style="34" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="64" t="s">
         <v>0</v>
       </c>
@@ -2824,7 +2889,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A2" s="16" t="s">
         <v>144</v>
       </c>
@@ -2835,7 +2900,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="16" t="s">
         <v>147</v>
       </c>
@@ -2846,7 +2911,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A4" s="16" t="s">
         <v>149</v>
       </c>
@@ -2857,7 +2922,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A5" s="16" t="s">
         <v>151</v>
       </c>
@@ -2882,17 +2947,17 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.85546875" customWidth="1"/>
-    <col min="2" max="2" width="18.140625" customWidth="1"/>
-    <col min="3" max="3" width="23.140625" customWidth="1"/>
-    <col min="4" max="4" width="17.140625" customWidth="1"/>
-    <col min="5" max="5" width="31.28515625" customWidth="1"/>
-    <col min="6" max="6" width="37.140625" customWidth="1"/>
+    <col min="1" max="1" width="11.83203125" customWidth="1"/>
+    <col min="2" max="2" width="18.1640625" customWidth="1"/>
+    <col min="3" max="3" width="23.1640625" customWidth="1"/>
+    <col min="4" max="4" width="17.1640625" customWidth="1"/>
+    <col min="5" max="5" width="31.33203125" customWidth="1"/>
+    <col min="6" max="6" width="37.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="61" t="s">
         <v>0</v>
       </c>
@@ -2912,7 +2977,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>159</v>
       </c>
@@ -2946,15 +3011,15 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="22.85546875" customWidth="1"/>
-    <col min="2" max="6" width="29.85546875" customWidth="1"/>
-    <col min="7" max="7" width="47.42578125" style="34" customWidth="1"/>
-    <col min="8" max="8" width="29.85546875" customWidth="1"/>
+    <col min="1" max="1" width="22.83203125" customWidth="1"/>
+    <col min="2" max="6" width="29.83203125" customWidth="1"/>
+    <col min="7" max="7" width="47.5" style="34" customWidth="1"/>
+    <col min="8" max="8" width="29.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="61" t="s">
         <v>0</v>
       </c>
@@ -2977,7 +3042,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="45" x14ac:dyDescent="0.2">
       <c r="A2" s="38" t="s">
         <v>164</v>
       </c>
@@ -2990,7 +3055,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="38" t="s">
         <v>166</v>
       </c>
@@ -3011,7 +3076,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="38" t="s">
         <v>168</v>
       </c>
@@ -3032,7 +3097,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="38" t="s">
         <v>170</v>
       </c>
@@ -3053,7 +3118,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="38" t="s">
         <v>172</v>
       </c>
@@ -3074,7 +3139,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="38" t="s">
         <v>174</v>
       </c>
@@ -3095,7 +3160,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="38" t="s">
         <v>175</v>
       </c>
@@ -3118,7 +3183,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="38" t="s">
         <v>176</v>
       </c>
@@ -3141,7 +3206,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="38" t="s">
         <v>177</v>
       </c>
@@ -3164,7 +3229,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="38" t="s">
         <v>178</v>
       </c>
@@ -3204,15 +3269,15 @@
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="29.42578125" defaultRowHeight="34.5" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="29.5" defaultRowHeight="34.5" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="34.7109375" customWidth="1"/>
-    <col min="2" max="3" width="17.140625" customWidth="1"/>
-    <col min="4" max="4" width="29.42578125" style="34"/>
+    <col min="1" max="1" width="34.6640625" customWidth="1"/>
+    <col min="2" max="3" width="17.1640625" customWidth="1"/>
+    <col min="4" max="4" width="29.5" style="34"/>
     <col min="5" max="5" width="66" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="34.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="65" t="s">
         <v>0</v>
       </c>
@@ -3229,7 +3294,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="131.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="131.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="53" t="s">
         <v>392</v>
       </c>
@@ -3246,7 +3311,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="363.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="363.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="53" t="s">
         <v>393</v>
       </c>
@@ -3263,7 +3328,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="222" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="222" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="53" t="s">
         <v>394</v>
       </c>
@@ -3280,7 +3345,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="288" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="288" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="53" t="s">
         <v>395</v>
       </c>
@@ -3297,7 +3362,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="128.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="128.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="53" t="s">
         <v>396</v>
       </c>
@@ -3330,13 +3395,13 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="23.42578125" defaultRowHeight="34.5" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="23.5" defaultRowHeight="34.5" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="4" max="4" width="42.85546875" style="34" customWidth="1"/>
-    <col min="5" max="5" width="67.42578125" customWidth="1"/>
+    <col min="4" max="4" width="42.83203125" style="34" customWidth="1"/>
+    <col min="5" max="5" width="67.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="34.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="65" t="s">
         <v>0</v>
       </c>
@@ -3353,7 +3418,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="233.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="233.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="53" t="s">
         <v>230</v>
       </c>
@@ -3370,7 +3435,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="312" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="312" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="53" t="s">
         <v>234</v>
       </c>
@@ -3387,7 +3452,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="126" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="126" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="53" t="s">
         <v>237</v>
       </c>
@@ -3404,7 +3469,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="305.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="305.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="53" t="s">
         <v>240</v>
       </c>
@@ -3421,7 +3486,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="135.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="135.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="53" t="s">
         <v>243</v>
       </c>
@@ -3438,7 +3503,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="354.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="354.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="53" t="s">
         <v>246</v>
       </c>
@@ -3455,7 +3520,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="228" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="228" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="53" t="s">
         <v>249</v>
       </c>
@@ -3472,7 +3537,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="373.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="373.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="53" t="s">
         <v>251</v>
       </c>
@@ -3489,7 +3554,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="116.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="116.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="53" t="s">
         <v>252</v>
       </c>
@@ -3522,16 +3587,16 @@
       <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="15.42578125" defaultRowHeight="39" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="15.5" defaultRowHeight="39" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="44.140625" customWidth="1"/>
-    <col min="6" max="6" width="35.7109375" customWidth="1"/>
-    <col min="7" max="7" width="21.85546875" customWidth="1"/>
+    <col min="1" max="1" width="44.1640625" customWidth="1"/>
+    <col min="6" max="6" width="35.6640625" customWidth="1"/>
+    <col min="7" max="7" width="21.83203125" customWidth="1"/>
     <col min="14" max="14" width="35" customWidth="1"/>
-    <col min="16" max="16" width="33.28515625" customWidth="1"/>
+    <col min="16" max="16" width="33.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="66" t="s">
         <v>0</v>
       </c>
@@ -3581,7 +3646,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="2" spans="1:16" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" ht="39" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="47" t="s">
         <v>203</v>
       </c>
@@ -3629,7 +3694,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="3" spans="1:16" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" ht="39" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="47" t="s">
         <v>211</v>
       </c>
@@ -3677,7 +3742,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="4" spans="1:16" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" ht="39" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="47" t="s">
         <v>213</v>
       </c>
@@ -3725,7 +3790,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="5" spans="1:16" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" ht="39" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="47" t="s">
         <v>216</v>
       </c>
@@ -3773,7 +3838,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="6" spans="1:16" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" ht="39" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="47" t="s">
         <v>218</v>
       </c>
@@ -3821,7 +3886,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="7" spans="1:16" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" ht="39" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="47" t="s">
         <v>220</v>
       </c>
@@ -3869,7 +3934,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="8" spans="1:16" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" ht="39" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="47" t="s">
         <v>222</v>
       </c>
@@ -3917,7 +3982,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="9" spans="1:16" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" ht="39" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="47" t="s">
         <v>404</v>
       </c>
@@ -3965,7 +4030,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="10" spans="1:16" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" ht="39" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="47" t="s">
         <v>192</v>
       </c>
@@ -4031,18 +4096,18 @@
       <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="18.7109375" customWidth="1"/>
-    <col min="2" max="2" width="29.85546875" customWidth="1"/>
-    <col min="3" max="3" width="29.7109375" customWidth="1"/>
-    <col min="4" max="4" width="26.5703125" customWidth="1"/>
-    <col min="5" max="5" width="12.28515625" customWidth="1"/>
-    <col min="6" max="6" width="29.7109375" customWidth="1"/>
-    <col min="7" max="7" width="113.42578125" customWidth="1"/>
+    <col min="1" max="1" width="18.6640625" customWidth="1"/>
+    <col min="2" max="2" width="29.83203125" customWidth="1"/>
+    <col min="3" max="3" width="29.6640625" customWidth="1"/>
+    <col min="4" max="4" width="26.5" customWidth="1"/>
+    <col min="5" max="5" width="12.33203125" customWidth="1"/>
+    <col min="6" max="6" width="29.6640625" customWidth="1"/>
+    <col min="7" max="7" width="113.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="66" t="s">
         <v>0</v>
       </c>
@@ -4065,7 +4130,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="47" t="s">
         <v>203</v>
       </c>
@@ -4078,7 +4143,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="47" t="s">
         <v>211</v>
       </c>
@@ -4099,7 +4164,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="47" t="s">
         <v>213</v>
       </c>
@@ -4120,7 +4185,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="47" t="s">
         <v>216</v>
       </c>
@@ -4141,7 +4206,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="47" t="s">
         <v>218</v>
       </c>
@@ -4162,7 +4227,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="47" t="s">
         <v>220</v>
       </c>
@@ -4185,7 +4250,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="47" t="s">
         <v>222</v>
       </c>
@@ -4208,7 +4273,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="47" t="s">
         <v>404</v>
       </c>
@@ -4245,16 +4310,16 @@
       <selection sqref="A1:O2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="25.5703125" customWidth="1"/>
-    <col min="5" max="5" width="13.5703125" customWidth="1"/>
-    <col min="6" max="6" width="13.85546875" customWidth="1"/>
-    <col min="12" max="12" width="14.42578125" customWidth="1"/>
-    <col min="13" max="13" width="35.85546875" customWidth="1"/>
+    <col min="2" max="2" width="25.5" customWidth="1"/>
+    <col min="5" max="5" width="13.5" customWidth="1"/>
+    <col min="6" max="6" width="13.83203125" customWidth="1"/>
+    <col min="12" max="12" width="14.5" customWidth="1"/>
+    <col min="13" max="13" width="35.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" s="78" t="s">
         <v>0</v>
       </c>
@@ -4301,7 +4366,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" s="79" t="s">
         <v>28</v>
       </c>
@@ -4358,15 +4423,15 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="17" customWidth="1"/>
-    <col min="2" max="2" width="18.7109375" customWidth="1"/>
-    <col min="3" max="3" width="44.5703125" customWidth="1"/>
-    <col min="4" max="6" width="18.7109375" customWidth="1"/>
+    <col min="2" max="2" width="18.6640625" customWidth="1"/>
+    <col min="3" max="3" width="44.5" customWidth="1"/>
+    <col min="4" max="6" width="18.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="62" t="s">
         <v>0</v>
       </c>
@@ -4377,7 +4442,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="13" t="s">
         <v>268</v>
       </c>
@@ -4388,7 +4453,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="13" t="s">
         <v>269</v>
       </c>
@@ -4399,7 +4464,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="13" t="s">
         <v>271</v>
       </c>
@@ -4426,15 +4491,15 @@
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="24" customWidth="1"/>
-    <col min="2" max="2" width="12.5703125" customWidth="1"/>
-    <col min="3" max="3" width="29.5703125" customWidth="1"/>
-    <col min="4" max="4" width="61.5703125" customWidth="1"/>
+    <col min="2" max="2" width="12.5" customWidth="1"/>
+    <col min="3" max="3" width="29.5" customWidth="1"/>
+    <col min="4" max="4" width="61.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
@@ -4448,7 +4513,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="11" t="s">
         <v>366</v>
       </c>
@@ -4458,7 +4523,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="11" t="s">
         <v>368</v>
       </c>
@@ -4470,7 +4535,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="11" t="s">
         <v>370</v>
       </c>
@@ -4482,7 +4547,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="11" t="s">
         <v>372</v>
       </c>
@@ -4509,15 +4574,15 @@
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="25.140625" customWidth="1"/>
-    <col min="2" max="4" width="12.140625" customWidth="1"/>
-    <col min="5" max="5" width="24.7109375" customWidth="1"/>
-    <col min="8" max="8" width="47.7109375" style="34" customWidth="1"/>
+    <col min="1" max="1" width="25.1640625" customWidth="1"/>
+    <col min="2" max="4" width="12.1640625" customWidth="1"/>
+    <col min="5" max="5" width="24.6640625" customWidth="1"/>
+    <col min="8" max="8" width="47.6640625" style="34" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="62" t="s">
         <v>272</v>
       </c>
@@ -4543,7 +4608,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="88" t="s">
         <v>439</v>
       </c>
@@ -4567,7 +4632,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="88" t="s">
         <v>437</v>
       </c>
@@ -4591,7 +4656,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="88" t="s">
         <v>438</v>
       </c>
@@ -4615,7 +4680,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="88" t="s">
         <v>440</v>
       </c>
@@ -4639,7 +4704,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="88" t="s">
         <v>441</v>
       </c>
@@ -4663,7 +4728,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="75.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="75.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="88" t="s">
         <v>444</v>
       </c>
@@ -4677,7 +4742,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="88" t="s">
         <v>443</v>
       </c>
@@ -4703,7 +4768,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="87" t="s">
         <v>462</v>
       </c>
@@ -4729,7 +4794,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="87" t="s">
         <v>442</v>
       </c>
@@ -4755,7 +4820,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="88" t="s">
         <v>435</v>
       </c>
@@ -4795,19 +4860,19 @@
       <selection sqref="A1:N17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="21" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="21" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="20.42578125" customWidth="1"/>
+    <col min="1" max="1" width="20.5" customWidth="1"/>
     <col min="2" max="2" width="25" customWidth="1"/>
     <col min="3" max="4" width="13" customWidth="1"/>
-    <col min="5" max="5" width="38.7109375" customWidth="1"/>
+    <col min="5" max="5" width="38.6640625" customWidth="1"/>
     <col min="6" max="8" width="13" customWidth="1"/>
-    <col min="9" max="9" width="42.85546875" customWidth="1"/>
-    <col min="13" max="13" width="37.140625" customWidth="1"/>
-    <col min="14" max="14" width="30.140625" customWidth="1"/>
+    <col min="9" max="9" width="42.83203125" customWidth="1"/>
+    <col min="13" max="13" width="37.1640625" customWidth="1"/>
+    <col min="14" max="14" width="30.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="30" t="s">
         <v>0</v>
       </c>
@@ -4851,7 +4916,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="88" t="s">
         <v>465</v>
       </c>
@@ -4893,7 +4958,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="3" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="88" t="s">
         <v>463</v>
       </c>
@@ -4935,7 +5000,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="88" t="s">
         <v>464</v>
       </c>
@@ -4977,7 +5042,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="5" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="88" t="s">
         <v>466</v>
       </c>
@@ -5019,7 +5084,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="6" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="90" t="s">
         <v>467</v>
       </c>
@@ -5061,7 +5126,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="7" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="90" t="s">
         <v>468</v>
       </c>
@@ -5103,7 +5168,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="90" t="s">
         <v>469</v>
       </c>
@@ -5145,7 +5210,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="90" t="s">
         <v>470</v>
       </c>
@@ -5187,7 +5252,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="10" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="90" t="s">
         <v>471</v>
       </c>
@@ -5229,7 +5294,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="11" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="90" t="s">
         <v>472</v>
       </c>
@@ -5271,7 +5336,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="12" spans="1:14" ht="167.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" ht="167.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="90" t="s">
         <v>476</v>
       </c>
@@ -5291,7 +5356,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="13" spans="1:14" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="90" t="s">
         <v>474</v>
       </c>
@@ -5335,7 +5400,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="14" spans="1:14" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="90" t="s">
         <v>473</v>
       </c>
@@ -5379,7 +5444,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="15" spans="1:14" ht="69" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" ht="69" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="88" t="s">
         <v>461</v>
       </c>
@@ -5423,7 +5488,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="16" spans="1:14" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="90" t="s">
         <v>475</v>
       </c>
@@ -5467,7 +5532,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="17" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="88" t="s">
         <v>477</v>
       </c>
@@ -5527,20 +5592,20 @@
       <selection activeCell="M18" sqref="M18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="19.5" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="19.5" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="26.7109375" customWidth="1"/>
-    <col min="2" max="4" width="13.140625" customWidth="1"/>
-    <col min="5" max="5" width="31.140625" customWidth="1"/>
-    <col min="6" max="7" width="13.140625" customWidth="1"/>
+    <col min="1" max="1" width="26.6640625" customWidth="1"/>
+    <col min="2" max="4" width="13.1640625" customWidth="1"/>
+    <col min="5" max="5" width="31.1640625" customWidth="1"/>
+    <col min="6" max="7" width="13.1640625" customWidth="1"/>
     <col min="8" max="8" width="13" customWidth="1"/>
-    <col min="9" max="9" width="60.28515625" customWidth="1"/>
-    <col min="13" max="13" width="30.140625" customWidth="1"/>
-    <col min="14" max="14" width="30.42578125" customWidth="1"/>
-    <col min="15" max="15" width="9.140625" style="92"/>
+    <col min="9" max="9" width="60.33203125" customWidth="1"/>
+    <col min="13" max="13" width="30.1640625" customWidth="1"/>
+    <col min="14" max="14" width="30.5" customWidth="1"/>
+    <col min="15" max="15" width="8.83203125" style="92"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="92" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" s="92" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="30" t="s">
         <v>0</v>
       </c>
@@ -5584,7 +5649,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="92" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" s="92" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="88" t="s">
         <v>448</v>
       </c>
@@ -5626,7 +5691,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="3" spans="1:14" s="92" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" s="92" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="88" t="s">
         <v>445</v>
       </c>
@@ -5668,7 +5733,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="4" spans="1:14" s="92" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" s="92" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="88" t="s">
         <v>446</v>
       </c>
@@ -5710,7 +5775,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="5" spans="1:14" s="92" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" s="92" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="88" t="s">
         <v>449</v>
       </c>
@@ -5752,7 +5817,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="6" spans="1:14" s="92" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" s="92" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="88" t="s">
         <v>450</v>
       </c>
@@ -5794,7 +5859,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="7" spans="1:14" s="92" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" s="92" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="88" t="s">
         <v>451</v>
       </c>
@@ -5836,7 +5901,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="8" spans="1:14" s="92" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" s="92" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="88" t="s">
         <v>452</v>
       </c>
@@ -5878,7 +5943,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="9" spans="1:14" s="92" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" s="92" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="88" t="s">
         <v>453</v>
       </c>
@@ -5920,7 +5985,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="10" spans="1:14" s="92" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" s="92" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="88" t="s">
         <v>454</v>
       </c>
@@ -5962,7 +6027,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="11" spans="1:14" s="92" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" s="92" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="88" t="s">
         <v>455</v>
       </c>
@@ -6004,7 +6069,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="12" spans="1:14" s="92" customFormat="1" ht="170.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" s="92" customFormat="1" ht="170.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="88" t="s">
         <v>459</v>
       </c>
@@ -6024,7 +6089,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="13" spans="1:14" s="92" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" s="92" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="88" t="s">
         <v>457</v>
       </c>
@@ -6068,7 +6133,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="14" spans="1:14" s="92" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" s="92" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="88" t="s">
         <v>456</v>
       </c>
@@ -6112,7 +6177,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="15" spans="1:14" s="92" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" s="92" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="88" t="s">
         <v>460</v>
       </c>
@@ -6156,7 +6221,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="16" spans="1:14" s="92" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" s="92" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="88" t="s">
         <v>458</v>
       </c>
@@ -6200,7 +6265,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="17" spans="1:14" s="92" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14" s="92" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="88" t="s">
         <v>447</v>
       </c>
@@ -6242,7 +6307,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="18" spans="1:14" s="92" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:14" s="92" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="88" t="s">
         <v>479</v>
       </c>
@@ -6300,14 +6365,14 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="25.5703125" customWidth="1"/>
-    <col min="2" max="2" width="32.28515625" customWidth="1"/>
-    <col min="3" max="3" width="44.42578125" customWidth="1"/>
+    <col min="1" max="1" width="25.5" customWidth="1"/>
+    <col min="2" max="2" width="32.33203125" customWidth="1"/>
+    <col min="3" max="3" width="44.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="62" t="s">
         <v>0</v>
       </c>
@@ -6318,7 +6383,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="13" t="s">
         <v>259</v>
       </c>
@@ -6329,7 +6394,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="13" t="s">
         <v>262</v>
       </c>
@@ -6340,7 +6405,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="13" t="s">
         <v>265</v>
       </c>
@@ -6367,15 +6432,15 @@
       <selection sqref="A1:P2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="6.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="52.140625" customWidth="1"/>
-    <col min="3" max="12" width="13.42578125" customWidth="1"/>
-    <col min="13" max="15" width="14.42578125" customWidth="1"/>
-    <col min="16" max="16" width="25.7109375" customWidth="1"/>
+    <col min="2" max="2" width="52.1640625" customWidth="1"/>
+    <col min="3" max="12" width="13.5" customWidth="1"/>
+    <col min="13" max="15" width="14.5" customWidth="1"/>
+    <col min="16" max="16" width="25.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A1" s="68" t="s">
         <v>0</v>
       </c>
@@ -6425,7 +6490,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="2" spans="1:16" ht="60" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A2" s="69" t="s">
         <v>36</v>
       </c>
@@ -6469,7 +6534,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A3" s="69" t="s">
         <v>40</v>
       </c>
@@ -6513,7 +6578,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4" s="69" t="s">
         <v>42</v>
       </c>
@@ -6557,7 +6622,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A5" s="69" t="s">
         <v>45</v>
       </c>
@@ -6601,7 +6666,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="6" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A6" s="69" t="s">
         <v>47</v>
       </c>
@@ -6645,7 +6710,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A7" s="69" t="s">
         <v>50</v>
       </c>
@@ -6689,7 +6754,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A8" s="69" t="s">
         <v>338</v>
       </c>
@@ -6733,7 +6798,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A9" s="69" t="s">
         <v>340</v>
       </c>
@@ -6777,7 +6842,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A10" s="69" t="s">
         <v>342</v>
       </c>
@@ -6821,7 +6886,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="11" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A11" s="69" t="s">
         <v>344</v>
       </c>
@@ -6865,7 +6930,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="12" spans="1:16" ht="165" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" ht="150" x14ac:dyDescent="0.2">
       <c r="A12" s="70" t="s">
         <v>345</v>
       </c>
@@ -6887,7 +6952,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="13" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" ht="30" x14ac:dyDescent="0.2">
       <c r="A13" s="70" t="s">
         <v>347</v>
       </c>
@@ -6933,7 +6998,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A14" s="70" t="s">
         <v>348</v>
       </c>
@@ -6979,7 +7044,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="15" spans="1:16" ht="60" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" ht="60" x14ac:dyDescent="0.2">
       <c r="A15" s="70" t="s">
         <v>349</v>
       </c>
@@ -7025,7 +7090,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="16" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" ht="30" x14ac:dyDescent="0.2">
       <c r="A16" s="70" t="s">
         <v>351</v>
       </c>
@@ -7084,20 +7149,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C10" sqref="A1:C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="22.140625" customWidth="1"/>
-    <col min="2" max="2" width="59.140625" customWidth="1"/>
-    <col min="8" max="8" width="15.7109375" customWidth="1"/>
-    <col min="10" max="10" width="24.140625" customWidth="1"/>
-    <col min="11" max="11" width="29.5703125" customWidth="1"/>
+    <col min="1" max="1" width="22.1640625" customWidth="1"/>
+    <col min="2" max="2" width="59.1640625" customWidth="1"/>
+    <col min="8" max="8" width="15.6640625" customWidth="1"/>
+    <col min="10" max="10" width="24.1640625" customWidth="1"/>
+    <col min="11" max="11" width="29.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" s="98" t="s">
         <v>0</v>
       </c>
@@ -7132,7 +7197,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" ht="46.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="100" t="s">
         <v>485</v>
       </c>
@@ -7165,7 +7230,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" ht="45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="100" t="s">
         <v>486</v>
       </c>
@@ -7198,7 +7263,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" ht="30" x14ac:dyDescent="0.2">
       <c r="A4" s="100" t="s">
         <v>487</v>
       </c>
@@ -7231,7 +7296,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" ht="30" x14ac:dyDescent="0.2">
       <c r="A5" s="100" t="s">
         <v>488</v>
       </c>
@@ -7264,7 +7329,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" ht="30" x14ac:dyDescent="0.2">
       <c r="A6" s="100" t="s">
         <v>489</v>
       </c>
@@ -7299,7 +7364,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" ht="30" x14ac:dyDescent="0.2">
       <c r="A7" s="100" t="s">
         <v>490</v>
       </c>
@@ -7332,7 +7397,7 @@
         <v>494</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" ht="30" x14ac:dyDescent="0.2">
       <c r="A8" s="100" t="s">
         <v>491</v>
       </c>
@@ -7365,7 +7430,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" ht="60" x14ac:dyDescent="0.2">
       <c r="A9" s="100" t="s">
         <v>493</v>
       </c>
@@ -7386,7 +7451,7 @@
         <v>506</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" ht="30" x14ac:dyDescent="0.2">
       <c r="A10" s="100" t="s">
         <v>507</v>
       </c>
@@ -7431,80 +7496,94 @@
 
 <file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="39.42578125" customWidth="1"/>
-    <col min="2" max="2" width="29.85546875" customWidth="1"/>
-    <col min="3" max="3" width="16.42578125" customWidth="1"/>
-    <col min="4" max="4" width="45.28515625" customWidth="1"/>
-    <col min="7" max="7" width="43.7109375" customWidth="1"/>
+    <col min="1" max="1" width="58.33203125" customWidth="1"/>
+    <col min="2" max="2" width="35.6640625" customWidth="1"/>
+    <col min="3" max="3" width="45" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="62" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="101" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="15" t="s">
-        <v>102</v>
-      </c>
-      <c r="C1" s="15" t="s">
-        <v>107</v>
-      </c>
-      <c r="D1" s="15" t="s">
-        <v>328</v>
-      </c>
-      <c r="E1" s="15" t="s">
-        <v>316</v>
-      </c>
-      <c r="F1" s="15" t="s">
-        <v>329</v>
-      </c>
-      <c r="G1" s="15" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="13" t="s">
-        <v>331</v>
-      </c>
-      <c r="B2" s="13" t="s">
-        <v>332</v>
-      </c>
-      <c r="C2" s="13" t="s">
-        <v>111</v>
-      </c>
-      <c r="D2" s="11"/>
-      <c r="E2" s="13" t="s">
-        <v>333</v>
-      </c>
-      <c r="F2" s="11"/>
-      <c r="G2" s="11" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="91.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="13" t="s">
-        <v>335</v>
-      </c>
-      <c r="B3" s="56" t="s">
-        <v>336</v>
-      </c>
-      <c r="C3" s="13" t="s">
-        <v>111</v>
-      </c>
-      <c r="D3" s="11"/>
-      <c r="E3" s="13" t="s">
-        <v>327</v>
-      </c>
-      <c r="F3" s="11"/>
-      <c r="G3" s="11" t="s">
-        <v>334</v>
+      <c r="B1" s="102" t="s">
+        <v>512</v>
+      </c>
+      <c r="C1" s="102" t="s">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="70" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="103" t="s">
+        <v>511</v>
+      </c>
+      <c r="B2" s="104" t="s">
+        <v>515</v>
+      </c>
+      <c r="C2" s="105" t="s">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="63" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="103" t="s">
+        <v>511</v>
+      </c>
+      <c r="B3" s="104" t="s">
+        <v>516</v>
+      </c>
+      <c r="C3" s="105" t="s">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="66" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="103" t="s">
+        <v>511</v>
+      </c>
+      <c r="B4" s="104" t="s">
+        <v>517</v>
+      </c>
+      <c r="C4" s="105" t="s">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="66" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="103" t="s">
+        <v>511</v>
+      </c>
+      <c r="B5" s="104" t="s">
+        <v>518</v>
+      </c>
+      <c r="C5" s="105" t="s">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="65" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="103" t="s">
+        <v>511</v>
+      </c>
+      <c r="B6" s="104" t="s">
+        <v>519</v>
+      </c>
+      <c r="C6" s="105" t="s">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="74" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="103" t="s">
+        <v>511</v>
+      </c>
+      <c r="B7" s="104" t="s">
+        <v>520</v>
+      </c>
+      <c r="C7" s="105" t="s">
+        <v>514</v>
       </c>
     </row>
   </sheetData>
@@ -7517,21 +7596,107 @@
 
 <file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="39.5" customWidth="1"/>
+    <col min="2" max="2" width="29.83203125" customWidth="1"/>
+    <col min="3" max="3" width="16.5" customWidth="1"/>
+    <col min="4" max="4" width="45.33203125" customWidth="1"/>
+    <col min="7" max="7" width="43.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" s="62" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="15" t="s">
+        <v>102</v>
+      </c>
+      <c r="C1" s="15" t="s">
+        <v>107</v>
+      </c>
+      <c r="D1" s="15" t="s">
+        <v>328</v>
+      </c>
+      <c r="E1" s="15" t="s">
+        <v>316</v>
+      </c>
+      <c r="F1" s="15" t="s">
+        <v>329</v>
+      </c>
+      <c r="G1" s="15" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" s="13" t="s">
+        <v>331</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>332</v>
+      </c>
+      <c r="C2" s="13" t="s">
+        <v>111</v>
+      </c>
+      <c r="D2" s="11"/>
+      <c r="E2" s="13" t="s">
+        <v>333</v>
+      </c>
+      <c r="F2" s="11"/>
+      <c r="G2" s="11" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="91.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="13" t="s">
+        <v>335</v>
+      </c>
+      <c r="B3" s="56" t="s">
+        <v>336</v>
+      </c>
+      <c r="C3" s="13" t="s">
+        <v>111</v>
+      </c>
+      <c r="D3" s="11"/>
+      <c r="E3" s="13" t="s">
+        <v>327</v>
+      </c>
+      <c r="F3" s="11"/>
+      <c r="G3" s="11" t="s">
+        <v>334</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A1" location="'Sheet names'!A1" display="TC No "/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="27.85546875" customWidth="1"/>
-    <col min="2" max="2" width="45.28515625" style="34" customWidth="1"/>
-    <col min="3" max="3" width="13.7109375" customWidth="1"/>
-    <col min="4" max="4" width="18.5703125" customWidth="1"/>
+    <col min="1" max="1" width="27.83203125" customWidth="1"/>
+    <col min="2" max="2" width="45.33203125" style="34" customWidth="1"/>
+    <col min="3" max="3" width="13.6640625" customWidth="1"/>
+    <col min="4" max="4" width="18.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="62" t="s">
         <v>0</v>
       </c>
@@ -7545,7 +7710,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="13" t="s">
         <v>126</v>
       </c>
@@ -7559,7 +7724,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="13" t="s">
         <v>129</v>
       </c>
@@ -7571,7 +7736,7 @@
       </c>
       <c r="D3" s="11"/>
     </row>
-    <row r="4" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="13" t="s">
         <v>132</v>
       </c>
@@ -7583,7 +7748,7 @@
       </c>
       <c r="D4" s="11"/>
     </row>
-    <row r="5" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="13" t="s">
         <v>325</v>
       </c>
@@ -7611,15 +7776,15 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="45.140625" customWidth="1"/>
-    <col min="2" max="2" width="23.85546875" customWidth="1"/>
-    <col min="13" max="13" width="27.140625" customWidth="1"/>
-    <col min="14" max="14" width="11.42578125" customWidth="1"/>
+    <col min="1" max="1" width="45.1640625" customWidth="1"/>
+    <col min="2" max="2" width="23.83203125" customWidth="1"/>
+    <col min="13" max="13" width="27.1640625" customWidth="1"/>
+    <col min="14" max="14" width="11.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" s="61" t="s">
         <v>0</v>
       </c>
@@ -7666,7 +7831,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>15</v>
       </c>
@@ -7709,7 +7874,7 @@
       <c r="N2" s="5"/>
       <c r="O2" s="5"/>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" s="7" t="s">
         <v>25</v>
       </c>
@@ -7752,7 +7917,7 @@
       <c r="N3" s="5"/>
       <c r="O3" s="5"/>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" s="7" t="s">
         <v>28</v>
       </c>
@@ -7812,15 +7977,15 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="20.7109375" customWidth="1"/>
+    <col min="1" max="1" width="20.6640625" customWidth="1"/>
     <col min="2" max="2" width="31" customWidth="1"/>
-    <col min="3" max="3" width="15.42578125" customWidth="1"/>
-    <col min="4" max="4" width="28.140625" customWidth="1"/>
+    <col min="3" max="3" width="15.5" customWidth="1"/>
+    <col min="4" max="4" width="28.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="64" t="s">
         <v>33</v>
       </c>
@@ -7834,7 +7999,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="90" t="s">
         <v>426</v>
       </c>
@@ -7848,7 +8013,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="90" t="s">
         <v>427</v>
       </c>
@@ -7860,7 +8025,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="90" t="s">
         <v>428</v>
       </c>
@@ -7872,7 +8037,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="90" t="s">
         <v>429</v>
       </c>
@@ -7882,7 +8047,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="90" t="s">
         <v>426</v>
       </c>
@@ -7912,21 +8077,21 @@
       <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="33" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="33" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="35.85546875" customWidth="1"/>
-    <col min="3" max="3" width="15.7109375" customWidth="1"/>
-    <col min="4" max="5" width="11.140625" customWidth="1"/>
-    <col min="6" max="6" width="18.5703125" customWidth="1"/>
-    <col min="7" max="7" width="16.7109375" customWidth="1"/>
+    <col min="2" max="2" width="35.83203125" customWidth="1"/>
+    <col min="3" max="3" width="15.6640625" customWidth="1"/>
+    <col min="4" max="5" width="11.1640625" customWidth="1"/>
+    <col min="6" max="6" width="18.5" customWidth="1"/>
+    <col min="7" max="7" width="16.6640625" customWidth="1"/>
     <col min="8" max="8" width="14" customWidth="1"/>
-    <col min="9" max="9" width="32.5703125" customWidth="1"/>
-    <col min="11" max="11" width="24.5703125" customWidth="1"/>
-    <col min="12" max="12" width="20.85546875" customWidth="1"/>
-    <col min="13" max="13" width="43.7109375" customWidth="1"/>
+    <col min="9" max="9" width="32.5" customWidth="1"/>
+    <col min="11" max="11" width="24.5" customWidth="1"/>
+    <col min="12" max="12" width="20.83203125" customWidth="1"/>
+    <col min="13" max="13" width="43.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" ht="33" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="63" t="s">
         <v>33</v>
       </c>
@@ -7967,7 +8132,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" ht="33" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="23" t="s">
         <v>70</v>
       </c>
@@ -8008,7 +8173,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" ht="33" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="23" t="s">
         <v>79</v>
       </c>
@@ -8049,7 +8214,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" ht="33" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="23" t="s">
         <v>83</v>
       </c>
@@ -8090,7 +8255,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" ht="33" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="23" t="s">
         <v>85</v>
       </c>
@@ -8149,14 +8314,14 @@
       <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="40.7109375" customWidth="1"/>
-    <col min="2" max="2" width="29.140625" customWidth="1"/>
-    <col min="3" max="3" width="28.85546875" customWidth="1"/>
+    <col min="1" max="1" width="40.6640625" customWidth="1"/>
+    <col min="2" max="2" width="29.1640625" customWidth="1"/>
+    <col min="3" max="3" width="28.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="63" t="s">
         <v>33</v>
       </c>
@@ -8167,7 +8332,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="23" t="s">
         <v>414</v>
       </c>
@@ -8176,7 +8341,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="47" t="s">
         <v>415</v>
       </c>
@@ -8187,7 +8352,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A4" s="47" t="s">
         <v>420</v>
       </c>
@@ -8215,15 +8380,15 @@
       <selection activeCell="P9" sqref="P9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="21" customWidth="1"/>
-    <col min="2" max="2" width="21.5703125" customWidth="1"/>
-    <col min="3" max="3" width="22.28515625" customWidth="1"/>
-    <col min="4" max="4" width="28.85546875" customWidth="1"/>
+    <col min="2" max="2" width="21.5" customWidth="1"/>
+    <col min="3" max="3" width="22.33203125" customWidth="1"/>
+    <col min="4" max="4" width="28.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="15" t="s">
         <v>377</v>
       </c>
@@ -8237,7 +8402,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="11" t="s">
         <v>381</v>
       </c>
@@ -8251,7 +8416,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="11" t="s">
         <v>383</v>
       </c>
@@ -8265,7 +8430,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="11" t="s">
         <v>385</v>
       </c>
@@ -8291,16 +8456,16 @@
       <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="28.28515625" customWidth="1"/>
-    <col min="2" max="2" width="22.5703125" customWidth="1"/>
-    <col min="3" max="3" width="13.7109375" customWidth="1"/>
+    <col min="1" max="1" width="28.33203125" customWidth="1"/>
+    <col min="2" max="2" width="22.5" customWidth="1"/>
+    <col min="3" max="3" width="13.6640625" customWidth="1"/>
     <col min="4" max="4" width="16" customWidth="1"/>
-    <col min="5" max="5" width="76.42578125" customWidth="1"/>
+    <col min="5" max="5" width="76.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="64" t="s">
         <v>0</v>
       </c>
@@ -8317,7 +8482,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="16" t="s">
         <v>91</v>
       </c>
@@ -8328,7 +8493,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="16" t="s">
         <v>93</v>
       </c>
@@ -8343,7 +8508,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="16" t="s">
         <v>97</v>
       </c>
@@ -8358,7 +8523,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="16" t="s">
         <v>99</v>
       </c>
@@ -8389,15 +8554,15 @@
       <selection sqref="A1:D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="20.140625" customWidth="1"/>
+    <col min="1" max="1" width="20.1640625" customWidth="1"/>
     <col min="2" max="2" width="39" customWidth="1"/>
     <col min="3" max="3" width="17" customWidth="1"/>
-    <col min="4" max="4" width="38.140625" customWidth="1"/>
+    <col min="4" max="4" width="38.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="86" t="s">
         <v>33</v>
       </c>
@@ -8411,7 +8576,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="13" t="s">
         <v>423</v>
       </c>
@@ -8425,7 +8590,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="83" t="s">
         <v>424</v>
       </c>
@@ -8439,7 +8604,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="83" t="s">
         <v>425</v>
       </c>
@@ -8453,7 +8618,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="83" t="s">
         <v>430</v>
       </c>
@@ -8467,7 +8632,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="83" t="s">
         <v>432</v>
       </c>
@@ -8481,7 +8646,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="83" t="s">
         <v>432</v>
       </c>

</xml_diff>